<commit_message>
Hood tech colors fix
</commit_message>
<xml_diff>
--- a/Excel/Hood/2022.02.18/25.02.2022 HOOD — техничка.xlsx
+++ b/Excel/Hood/2022.02.18/25.02.2022 HOOD — техничка.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUH\Documents\HatsAndCaps\Excel\Hood\2022.02.18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{782CB79E-37CD-45F8-9B18-73F6C57E6C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{99277F8E-80F6-4D3F-BC49-5FC24A91AB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B897EB2-BCC8-4CF7-B173-73EC4B458CC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D503BA80-60C4-4BF5-B22C-98CC006DD3F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Техничка HOOD" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
     <t>черный / красный</t>
   </si>
   <si>
-    <t>92-022-12</t>
+    <t>92-022-65</t>
   </si>
   <si>
     <t>100-MWL005-CO005-MN</t>
@@ -414,7 +414,7 @@
     <t>Maroon</t>
   </si>
   <si>
-    <t>бордовый / белый</t>
+    <t>бордовый / голубой</t>
   </si>
   <si>
     <t>92-023-08</t>
@@ -624,7 +624,7 @@
     <t>Khaki</t>
   </si>
   <si>
-    <t>кремовый / коричневый</t>
+    <t>бежевый / коричневый</t>
   </si>
   <si>
     <t>92-041-83</t>
@@ -1043,7 +1043,7 @@
         <xdr:cNvPr id="2" name="Рисунок 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28D5AAD8-E907-447E-8FF7-A8E3238163B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ADCEC43-761B-4F8F-AFD0-06D423D689CB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1093,7 +1093,7 @@
         <xdr:cNvPr id="3" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09955B5D-2831-46FD-B003-299B999C02CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{193722A1-383A-4943-96C2-1070C0F433FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1143,7 +1143,7 @@
         <xdr:cNvPr id="4" name="Рисунок 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62D38C92-3B17-41DA-B596-98BB7EAECD9A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29E95A06-19B5-41B6-BC71-CD7B509D46EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1193,7 +1193,7 @@
         <xdr:cNvPr id="5" name="Рисунок 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{137518D2-F006-4B4E-BD30-20F3D5E2B4C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F2F0BC8-1794-4F7C-B2DE-4A2C52895CED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1243,7 +1243,7 @@
         <xdr:cNvPr id="6" name="Рисунок 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC2E7FFB-F061-4443-AEFD-E52542021078}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FDCBBE9-6B22-4042-AD5D-C69F5EF72390}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1293,7 +1293,7 @@
         <xdr:cNvPr id="7" name="Рисунок 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B9BB521-F2C6-4179-99BD-71A152C8575E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC22F3B4-7CE1-4266-8DF6-CB8AB6F37A19}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1343,7 +1343,7 @@
         <xdr:cNvPr id="8" name="Рисунок 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F18B9195-81D0-43E9-AC2B-3FA67E3F716D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A29042C8-542E-4538-A11C-253A1284BF40}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1393,7 +1393,7 @@
         <xdr:cNvPr id="9" name="Рисунок 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC2B694A-0210-4CBD-A8B8-E3341F1F06F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4764DE55-2B10-4409-8FBC-ECCBD6B7042A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1443,7 +1443,7 @@
         <xdr:cNvPr id="10" name="Рисунок 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{009C8789-ADE2-42D3-B059-D84D53EFA8EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D269C5E-723D-4EAA-8873-808CF2258A3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1493,7 +1493,7 @@
         <xdr:cNvPr id="11" name="Рисунок 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{960EAB8A-4303-4316-9337-BAC468195F5F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C6D4D31-F416-48D8-A43B-18C912E8C97B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1543,7 +1543,7 @@
         <xdr:cNvPr id="12" name="Рисунок 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09D4C5CC-4480-447B-B39A-DAE2732C60F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08873A45-ADAA-4BD7-9180-18C624134879}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1593,7 +1593,7 @@
         <xdr:cNvPr id="13" name="Рисунок 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06D50767-EDD9-4B53-AA66-1310A8C9BA0E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AFBDED1-0E4F-4FB5-90C6-C3F7CB8F5297}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1643,7 +1643,7 @@
         <xdr:cNvPr id="14" name="Рисунок 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C22AC9FF-7E7F-42C3-8EB8-82C9E502CD91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAF82C61-470D-4A82-BA3B-804EF38F2423}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1693,7 +1693,7 @@
         <xdr:cNvPr id="15" name="Рисунок 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{097FFFE1-2529-4E10-BCBE-2F593704E86F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32070505-EC6C-4864-9A8A-6B55F08D8649}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1743,7 +1743,7 @@
         <xdr:cNvPr id="16" name="Рисунок 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{861DA257-36F3-46A4-8E4E-C1B706FAA303}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D278F4D5-155B-4C90-95D3-F797401FA5E2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1793,7 +1793,7 @@
         <xdr:cNvPr id="17" name="Рисунок 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A230A8F-14D3-463E-9835-FC5B413539FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8958DBBF-9805-4802-B946-7190911C1803}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1843,7 +1843,7 @@
         <xdr:cNvPr id="18" name="Рисунок 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85D1DA84-E1BC-4387-B407-E9DA1E329151}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBFA03A9-EC9E-4990-9F0A-4D5190AEFE25}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1893,7 +1893,7 @@
         <xdr:cNvPr id="19" name="Рисунок 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBFC9A55-A792-4639-8008-164E9B3CBF30}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E4483A-83D3-480E-81C0-EFDA99159C2B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1943,7 +1943,7 @@
         <xdr:cNvPr id="20" name="Рисунок 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{983F3055-5506-4F1D-A00E-1F6327E3326C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C338833A-13FC-4607-8A2D-45ED38ABDACF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1993,7 +1993,7 @@
         <xdr:cNvPr id="21" name="Рисунок 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DBC289F-33CD-415B-B80A-392C10F9E4DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B181BBBE-1BCD-4F53-87DE-98E2176B5046}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2043,7 +2043,7 @@
         <xdr:cNvPr id="22" name="Рисунок 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E945C894-2AE2-4FC2-9B41-869FAD2228AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81BEB382-8AD4-4714-A298-6DECDCEF6CED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2093,7 +2093,7 @@
         <xdr:cNvPr id="23" name="Рисунок 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC44708B-A2EC-42BD-B0A1-215B5A5F8CBF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7B6F95E-DE3B-4079-B217-DDD3268AC853}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2143,7 +2143,7 @@
         <xdr:cNvPr id="24" name="Рисунок 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AE95B47-4BA1-457F-91A0-62A782D0BCF2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53738653-4D4E-4EE8-AB4A-ABE151CEAD5D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2193,7 +2193,7 @@
         <xdr:cNvPr id="25" name="Рисунок 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69151517-24FB-4548-A9B9-0BBD06BED381}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A55956DA-2606-4078-BE04-848E858A1B4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2243,7 +2243,7 @@
         <xdr:cNvPr id="26" name="Рисунок 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7887F9B3-06A7-4238-B1FC-5887F3643D8C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE35BED-81DD-4349-A38F-90DF95556BFC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2293,7 +2293,7 @@
         <xdr:cNvPr id="27" name="Рисунок 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38B55A8A-1E8E-45AD-ADD0-40C415907DD1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48F30EB0-7E63-4EE7-9397-031657D0B90A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2343,7 +2343,7 @@
         <xdr:cNvPr id="28" name="Рисунок 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2258FFFD-A992-4B53-8B8F-8932EC599E5A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E651EE5-5C56-4E3B-9ED1-D27A948DE6E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2393,7 +2393,7 @@
         <xdr:cNvPr id="29" name="Рисунок 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5492C3DE-154D-4256-AA8C-F8103A82BDF3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45D5A75B-BED5-4DFA-ABF5-29A39D7345ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2443,7 +2443,7 @@
         <xdr:cNvPr id="30" name="Рисунок 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79AF44DF-8464-49DA-88AE-577F1F8B2B89}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C866795B-B0CF-400A-A605-08B5F380D624}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2493,7 +2493,7 @@
         <xdr:cNvPr id="31" name="Рисунок 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15ED18C4-BF98-4415-A3AB-67BD58C2DC08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB1863BA-B489-45F7-AE86-7685D3220DCB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2543,7 +2543,7 @@
         <xdr:cNvPr id="32" name="Рисунок 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1654B797-A83F-4EBB-A7D6-F118603CE1EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F036A1F-5D00-44A1-8BFA-17CCF7D83204}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2593,7 +2593,7 @@
         <xdr:cNvPr id="33" name="Рисунок 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5C8BA7-455B-439A-8283-A0A2A98F08CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD99587E-3819-44C1-AD0E-9782712A6679}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2643,7 +2643,7 @@
         <xdr:cNvPr id="34" name="Рисунок 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2911013A-5C08-48EE-BE38-A87D6718FE62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38C5DD04-D02F-45F4-A8F7-7EDF5CC2A015}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2693,7 +2693,7 @@
         <xdr:cNvPr id="35" name="Рисунок 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6D57489-9A07-4D94-8059-D73D738F217C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DD546B3-C5FF-4096-AA74-BBE1C3040275}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2743,7 +2743,7 @@
         <xdr:cNvPr id="36" name="Рисунок 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C080652-5C61-4415-AC10-FC561F3BB3CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F6BC124-0ADF-4B90-B57F-D9F8576CE6D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2793,7 +2793,7 @@
         <xdr:cNvPr id="37" name="Рисунок 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAEC5A74-58B6-4AB2-A0BE-58B8BC832270}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09572FA3-4322-41E8-AD7A-DFF427D0ABF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2843,7 +2843,7 @@
         <xdr:cNvPr id="38" name="Рисунок 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2593085E-4F2B-47A9-A331-ABADAF975710}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20691E11-DF47-4CBF-B2C2-AC7CA7426144}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2893,7 +2893,7 @@
         <xdr:cNvPr id="39" name="Рисунок 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AD85674-216E-42DB-921D-477A872EE3E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEEAC71B-4BF5-437E-B444-5818105C9629}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2943,7 +2943,7 @@
         <xdr:cNvPr id="40" name="Рисунок 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B48373CB-4222-469E-91FD-353F5242A629}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0CFAD7F-27FE-4B62-B680-392316A46B52}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2993,7 +2993,7 @@
         <xdr:cNvPr id="41" name="Рисунок 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94CBDEFC-30E1-490F-8E6E-211BAE596439}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76A15DCC-E6BE-400D-B395-22B540B6FEBE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3043,7 +3043,7 @@
         <xdr:cNvPr id="42" name="Рисунок 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5F72F35-8934-45E0-870C-9641780CAEBC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0821247-D1D2-40EE-8277-EAE0DFAB0CD0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3093,7 +3093,7 @@
         <xdr:cNvPr id="43" name="Рисунок 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF6CAE89-F687-458C-B51A-E749149527E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{103151FE-7DA3-456D-BFAB-24EBBF653465}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3143,7 +3143,7 @@
         <xdr:cNvPr id="44" name="Рисунок 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D12BB098-A1BA-4839-B052-A69AE161577A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12B8E054-B9FC-454D-8D37-BB3F6AD715D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3193,7 +3193,7 @@
         <xdr:cNvPr id="45" name="Рисунок 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC293EAE-41FE-4C6B-80E2-0C42BEBC2072}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3D0E8AC-0529-478A-B1CF-730BA9BBE135}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3243,7 +3243,7 @@
         <xdr:cNvPr id="46" name="Рисунок 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE343FBF-49F5-426E-8B12-EEA38D49665D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA510986-F745-4909-8AF8-E39A757DC396}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3293,7 +3293,7 @@
         <xdr:cNvPr id="47" name="Рисунок 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBAB457C-53F3-44F3-9951-758C83E601CF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7135C2A4-5DC5-4396-9C79-375650CDB2CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3343,7 +3343,7 @@
         <xdr:cNvPr id="48" name="Рисунок 47">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C93DC1D-0016-4493-8A43-59107FDD5288}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16FFF085-85B9-4B98-A598-A7F911AFF1A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3393,7 +3393,7 @@
         <xdr:cNvPr id="49" name="Рисунок 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{557D55E0-B937-4E8C-A3F0-E464700712CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E99E09A-C085-4674-9501-03ABF2A4C287}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3443,7 +3443,7 @@
         <xdr:cNvPr id="50" name="Рисунок 49">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7394D3E7-22EA-4131-B481-27BC68DD0DFE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8583069-6C2A-44F8-BC56-02C7C56370E0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3493,7 +3493,7 @@
         <xdr:cNvPr id="51" name="Рисунок 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{966536F3-30FA-44CB-A9BD-29B1154DA275}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12D8F433-2EFA-4642-BB37-8D32AEBB3B46}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3824,14 +3824,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA82E27-13A7-419A-BB75-79D64F0D4B54}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21177459-E830-4111-84C6-66DD96A878E9}">
   <sheetPr codeName="Лист9">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:BD153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="BC1" sqref="BC1:BC1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>